<commit_message>
commit final - ajustado al diagrama
</commit_message>
<xml_diff>
--- a/backend/src/output/vinos.xlsx
+++ b/backend/src/output/vinos.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="24">
   <si>
     <t>Puntaje</t>
   </si>
@@ -28,67 +28,61 @@
     <t>Precio</t>
   </si>
   <si>
+    <t>Finca Altamira</t>
+  </si>
+  <si>
+    <t>Bodega Norton</t>
+  </si>
+  <si>
+    <t>["Malbec Reserva - Tipo Uva: Malbec","Cabernet Sauvignon Gran Reserva - Tipo Uva: Cabernet Sauvignon"]</t>
+  </si>
+  <si>
+    <t>Estrellas Blend</t>
+  </si>
+  <si>
+    <t>Bodega El Esteco</t>
+  </si>
+  <si>
+    <t>["Malbec Reserva - Tipo Uva: Malbec","Syrah Premium - Tipo Uva: Syrah"]</t>
+  </si>
+  <si>
+    <t>Cumbres Malbec</t>
+  </si>
+  <si>
+    <t>["Malbec Reserva - Tipo Uva: Malbec"]</t>
+  </si>
+  <si>
+    <t>Viña de las Estrellas</t>
+  </si>
+  <si>
+    <t>Trapiche Merlot</t>
+  </si>
+  <si>
+    <t>Bodega Trapiche</t>
+  </si>
+  <si>
+    <t>["Merlot Reserva Especial - Tipo Uva: Merlot"]</t>
+  </si>
+  <si>
     <t>Norton Malbec Especial</t>
   </si>
   <si>
-    <t>{"nombre":"Bodega Norton","region":{"nombre":"Valle de Uco"}}</t>
-  </si>
-  <si>
-    <t>["Malbec Reserva - Tipo Uva: Malbec"]</t>
-  </si>
-  <si>
     <t>Cabernet de Trapiche</t>
   </si>
   <si>
-    <t>{"nombre":"Bodega Trapiche","region":{"nombre":"Maipú"}}</t>
-  </si>
-  <si>
     <t>["Cabernet Sauvignon Gran Reserva - Tipo Uva: Cabernet Sauvignon"]</t>
   </si>
   <si>
-    <t>Viña de las Estrellas</t>
-  </si>
-  <si>
-    <t>Finca Altamira</t>
-  </si>
-  <si>
-    <t>["Malbec Reserva - Tipo Uva: Malbec","Cabernet Sauvignon Gran Reserva - Tipo Uva: Cabernet Sauvignon"]</t>
-  </si>
-  <si>
-    <t>Esteco Syrah</t>
-  </si>
-  <si>
-    <t>{"nombre":"Bodega El Esteco","region":{"nombre":"Tulum"}}</t>
-  </si>
-  <si>
-    <t>["Syrah Premium - Tipo Uva: Syrah"]</t>
-  </si>
-  <si>
-    <t>Colección Privada</t>
-  </si>
-  <si>
     <t>Blend de Valle</t>
   </si>
   <si>
     <t>["Malbec Reserva - Tipo Uva: Malbec","Merlot Reserva Especial - Tipo Uva: Merlot"]</t>
   </si>
   <si>
-    <t>Famatina Chardonnay</t>
-  </si>
-  <si>
-    <t>{"nombre":"Bodega La Riojana","region":{"nombre":"Famatina"}}</t>
-  </si>
-  <si>
-    <t>["Chardonnay Select - Tipo Uva: Chardonnay"]</t>
-  </si>
-  <si>
-    <t>Gran Malbec de Norton</t>
-  </si>
-  <si>
-    <t>Estrellas Blend</t>
-  </si>
-  <si>
-    <t>["Malbec Reserva - Tipo Uva: Malbec","Syrah Premium - Tipo Uva: Syrah"]</t>
+    <t>Norton Reserva</t>
+  </si>
+  <si>
+    <t>Altura Malbec</t>
   </si>
 </sst>
 </file>
@@ -468,7 +462,9 @@
   <dimension ref="A1:E11"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
-    <col min="1" max="5" width="10" customWidth="1"/>
+    <col min="1" max="1" width="10" customWidth="1"/>
+    <col min="2" max="4" width="20" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -490,7 +486,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B2" t="s">
         <v>5</v>
@@ -502,12 +498,12 @@
         <v>7</v>
       </c>
       <c r="E2">
-        <v>5500</v>
+        <v>7200</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>81</v>
+        <v>94.5</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
@@ -519,12 +515,12 @@
         <v>10</v>
       </c>
       <c r="E3">
-        <v>4300</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>78</v>
+        <v>80.5</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
@@ -533,32 +529,32 @@
         <v>6</v>
       </c>
       <c r="D4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E4">
-        <v>8000</v>
+        <v>4800</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>75</v>
+        <v>63</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C5" t="s">
         <v>6</v>
       </c>
       <c r="D5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="E5">
-        <v>7200</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>68.5</v>
+        <v>61.43</v>
       </c>
       <c r="B6" t="s">
         <v>14</v>
@@ -570,12 +566,12 @@
         <v>16</v>
       </c>
       <c r="E6">
-        <v>5000</v>
+        <v>3200</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>68</v>
+        <v>60.67</v>
       </c>
       <c r="B7" t="s">
         <v>17</v>
@@ -584,78 +580,78 @@
         <v>6</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E7">
-        <v>8500</v>
+        <v>5500</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>66.5</v>
+        <v>60</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="D8" t="s">
         <v>19</v>
       </c>
       <c r="E8">
-        <v>6500</v>
+        <v>4300</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>66</v>
+        <v>58.6</v>
       </c>
       <c r="B9" t="s">
         <v>20</v>
       </c>
       <c r="C9" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" t="s">
         <v>21</v>
       </c>
-      <c r="D9" t="s">
-        <v>22</v>
-      </c>
       <c r="E9">
-        <v>5400</v>
+        <v>6500</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>63</v>
+        <v>50.67</v>
       </c>
       <c r="B10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C10" t="s">
         <v>6</v>
       </c>
       <c r="D10" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E10">
-        <v>7000</v>
+        <v>7500</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>62</v>
+        <v>49.33</v>
       </c>
       <c r="B11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" t="s">
-        <v>15</v>
+        <v>6</v>
       </c>
       <c r="D11" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E11">
-        <v>6500</v>
+        <v>4200</v>
       </c>
     </row>
   </sheetData>

</xml_diff>